<commit_message>
added first results to table
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailunipaderbornde-my.sharepoint.com/personal/chschaef_mail_uni-paderborn_de/Documents/Studium/Master/4. Semester/Master thesis/repository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="11_AD4DB114E441178AC67DF47A1E96CFBE693EDF24" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94C550B5-2EA7-41BB-8E53-440E560DA940}"/>
+  <xr:revisionPtr revIDLastSave="171" documentId="11_AD4DB114E441178AC67DF47A1E96CFBE693EDF24" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D87AE1AF-70C3-473E-9102-0DA8979BEF57}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -283,34 +283,34 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -595,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -621,31 +621,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="19" t="s">
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="22" t="s">
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
     </row>
     <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -716,14 +716,41 @@
       <c r="E3" s="8">
         <v>1000</v>
       </c>
+      <c r="F3" s="8">
+        <v>1.8585000000000001E-2</v>
+      </c>
+      <c r="G3" s="8">
+        <v>123.25945299999999</v>
+      </c>
+      <c r="H3" s="8">
+        <v>1.4371999999999999E-2</v>
+      </c>
       <c r="I3" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="9">
         <v>1000</v>
       </c>
+      <c r="K3" s="9">
+        <v>2.0653000000000001E-2</v>
+      </c>
+      <c r="L3" s="9">
+        <v>123.334343</v>
+      </c>
+      <c r="M3" s="9">
+        <v>1.7398E-2</v>
+      </c>
       <c r="N3" s="6">
         <v>5000</v>
+      </c>
+      <c r="O3" s="6">
+        <v>2.0920999999999999E-2</v>
+      </c>
+      <c r="P3" s="6">
+        <v>123.322998</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>1.5885E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactoring: UncertaintySampler + -Measures
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailunipaderbornde-my.sharepoint.com/personal/chschaef_mail_uni-paderborn_de/Documents/Studium/Master/4. Semester/Master thesis/repository/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\OneDrive\OneDrive - mail.uni-paderborn.de\Studium\Master\4. Semester\Master thesis\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="322" documentId="11_AD4DB114E441178AC67DF47A1E96CFBE693EDF24" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01E92341-4266-4C83-9F34-7831EC64A6D2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97D90E0-9EF2-4584-A98F-F1FAEA670405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>2022.02.06.115931_gan_train_distmult_transe_wn18rr</t>
+  </si>
+  <si>
+    <t>Uncertainty Sampling Entropy Max Distribution</t>
   </si>
 </sst>
 </file>
@@ -439,50 +445,11 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -530,6 +497,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -948,16 +954,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.88671875" style="8" bestFit="1" customWidth="1"/>
@@ -976,169 +982,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
     </row>
     <row r="2" spans="1:17" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="36"/>
-      <c r="B2" s="26" t="s">
+      <c r="A2" s="23"/>
+      <c r="B2" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="26" t="s">
+      <c r="C2" s="48"/>
+      <c r="D2" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="26" t="s">
+      <c r="E2" s="48"/>
+      <c r="F2" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
       <c r="K2"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
     </row>
     <row r="3" spans="1:17" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
     </row>
     <row r="4" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="41" t="s">
+      <c r="C4" s="27"/>
+      <c r="D4" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="40"/>
-      <c r="F4" s="39" t="s">
+      <c r="E4" s="27"/>
+      <c r="F4" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="42"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
     </row>
     <row r="5" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="41" t="s">
+      <c r="C5" s="27"/>
+      <c r="D5" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="40"/>
-      <c r="F5" s="39" t="s">
+      <c r="E5" s="27"/>
+      <c r="F5" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="42"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
     </row>
     <row r="6" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
     </row>
     <row r="7" spans="1:17" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
       <c r="H7"/>
       <c r="I7"/>
       <c r="J7"/>
@@ -1151,15 +1157,15 @@
       <c r="Q7"/>
     </row>
     <row r="8" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
       <c r="H8"/>
       <c r="I8"/>
       <c r="J8"/>
@@ -1172,15 +1178,15 @@
       <c r="Q8"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
       <c r="H9"/>
       <c r="I9"/>
       <c r="J9"/>
@@ -1193,15 +1199,15 @@
       <c r="Q9"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
       <c r="H10"/>
       <c r="I10"/>
       <c r="J10"/>
@@ -1214,15 +1220,15 @@
       <c r="Q10"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
       <c r="H11"/>
       <c r="I11"/>
       <c r="J11"/>
@@ -1235,15 +1241,15 @@
       <c r="Q11"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
       <c r="H12"/>
       <c r="I12"/>
       <c r="J12"/>
@@ -1256,15 +1262,15 @@
       <c r="Q12"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
       <c r="H13"/>
       <c r="I13"/>
       <c r="J13"/>
@@ -1289,7 +1295,7 @@
       <c r="H14"/>
       <c r="I14"/>
       <c r="J14"/>
-      <c r="K14" s="24" t="s">
+      <c r="K14" s="14" t="s">
         <v>26</v>
       </c>
       <c r="L14">
@@ -1347,7 +1353,7 @@
       <c r="P16"/>
       <c r="Q16"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -1366,34 +1372,34 @@
       <c r="P17"/>
       <c r="Q17"/>
     </row>
-    <row r="18" spans="1:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="A18" s="22" t="s">
+    <row r="18" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A18" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="19" t="s">
+      <c r="B18" s="45"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="16" t="s">
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="14" t="s">
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-    </row>
-    <row r="19" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
+    </row>
+    <row r="19" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -1446,7 +1452,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>44517</v>
       </c>
@@ -1497,6 +1503,26 @@
       </c>
       <c r="Q20" s="7">
         <v>1.5885E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>44598</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="R21" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>